<commit_message>
Update - Comparando fornecedores - Gráfico
Melhorando o gráfico
</commit_message>
<xml_diff>
--- a/Aula 4 - Atividade 05 - Comparando fornecedor - Grafico.xlsx
+++ b/Aula 4 - Atividade 05 - Comparando fornecedor - Grafico.xlsx
@@ -105,7 +105,7 @@
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:rPr>
-              <a:t>Qtd_Vendas_NebulaNetworks, Qtd_Vendas_HorizonDistributors e Qtd_Vendas_AstroSupply</a:t>
+              <a:t>COMPARATIVO DE VENDAS</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -119,9 +119,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'Comparando dados'!$B$1</c:f>
-            </c:strRef>
+            <c:v>Nebula Networks</c:v>
           </c:tx>
           <c:spPr>
             <a:ln cmpd="sng">
@@ -150,9 +148,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'Comparando dados'!$C$1</c:f>
-            </c:strRef>
+            <c:v>Horizon Distributors</c:v>
           </c:tx>
           <c:spPr>
             <a:ln cmpd="sng">
@@ -181,9 +177,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'Comparando dados'!$D$1</c:f>
-            </c:strRef>
+            <c:v>Astro Supply</c:v>
           </c:tx>
           <c:spPr>
             <a:ln cmpd="sng">
@@ -208,11 +202,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1444254018"/>
-        <c:axId val="1309618337"/>
+        <c:axId val="2087400262"/>
+        <c:axId val="1094825286"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1444254018"/>
+        <c:axId val="2087400262"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -239,7 +233,7 @@
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                   </a:rPr>
-                  <a:t>Ano/Mes</a:t>
+                  <a:t>Periodo</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -264,10 +258,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1309618337"/>
+        <c:crossAx val="1094825286"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1309618337"/>
+        <c:axId val="1094825286"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -300,7 +294,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr lvl="0">
-                  <a:defRPr b="0">
+                  <a:defRPr b="1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -308,13 +302,13 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0">
+                  <a:rPr b="1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                   </a:rPr>
-                  <a:t/>
+                  <a:t>Quantidade de vendas</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -342,7 +336,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1444254018"/>
+        <c:crossAx val="2087400262"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -377,7 +371,7 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="7505700" cy="4648200"/>
+    <xdr:ext cx="7524750" cy="4648200"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="1" name="Chart 1" title="Gráfico"/>

</xml_diff>